<commit_message>
Added Beta test 2 email request
</commit_message>
<xml_diff>
--- a/Documentation/Beta Test Feedback/Beta test feedback summary.xlsx
+++ b/Documentation/Beta Test Feedback/Beta test feedback summary.xlsx
@@ -500,12 +500,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="249.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>

</xml_diff>